<commit_message>
Added title with timestamp to each sheet.
</commit_message>
<xml_diff>
--- a/Internet_pricing_All_2022-08-08.xlsx
+++ b/Internet_pricing_All_2022-08-08.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>FUJI</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>Tape&amp;Media</t>
+  </si>
+  <si>
+    <t>LTO7 Internet Pricing as of 2022-08-08</t>
+  </si>
+  <si>
+    <t>LTO8 Internet Pricing as of 2022-08-08</t>
+  </si>
+  <si>
+    <t>LTO9 Internet Pricing as of 2022-08-08</t>
   </si>
 </sst>
 </file>
@@ -398,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,6 +417,11 @@
     <col min="2" max="5" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2" spans="1:5">
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -480,7 +494,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -490,6 +504,11 @@
     <col min="2" max="5" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="2" spans="1:5">
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -562,7 +581,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -572,6 +591,11 @@
     <col min="2" max="5" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="2" spans="1:5">
       <c r="B2" s="2" t="s">
         <v>0</v>

</xml_diff>